<commit_message>
Comecando a aplicacao da funcionalidade de cadastro, alteracao e exclusao da receita
</commit_message>
<xml_diff>
--- a/documentacao/dinheiroNoBolso.xlsx
+++ b/documentacao/dinheiroNoBolso.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>Projeto Dinheiro no Bolso (Aplicativo Android)</t>
   </si>
@@ -119,9 +119,6 @@
     <t>DBRECEITANOME</t>
   </si>
   <si>
-    <t>DBRECEITATIPO</t>
-  </si>
-  <si>
     <t>DBRECEITAVALOR</t>
   </si>
   <si>
@@ -165,6 +162,30 @@
  `DBDESPESAVALOR` REAL NOT NULL,
  `DBDESPESADATAVENC` TEXT NOT NULL,
  `DBDESPESASTATUS` INTEGER NOT NULL
+);</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">DBRECEITATIPO </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Receita Salário = 0 e Variável = 1)</t>
+    </r>
+  </si>
+  <si>
+    <t>Script:                                                                                                                                                                                         CREATE TABLE `DBRECEITAS` (
+ `DBRECEITAID` INTEGER NOT NULL PRIMARY KEY AUTOINCREMENT,
+ `DBRECEITANOME` TEXT NOT NULL,
+ `DBRECEITATIPO` INTEGER NOT NULL,
+ `DBRECEITAVALOR` REAL NOT NULL,
+ `DBRECEITADATARECEBIMENTO` TEXT NOT NULL
 );</t>
   </si>
 </sst>
@@ -732,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1024"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:L12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,7 +801,7 @@
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -866,7 +887,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="9"/>
@@ -920,7 +941,7 @@
         <v>29</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="9"/>
@@ -953,15 +974,17 @@
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
+      <c r="D13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
@@ -969,15 +992,15 @@
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -987,15 +1010,15 @@
         <v>18</v>
       </c>
       <c r="C15" s="10"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1005,15 +1028,15 @@
         <v>32</v>
       </c>
       <c r="C16" s="9"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -1023,69 +1046,69 @@
         <v>33</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C18" s="8"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="9"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="9"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D21" s="5"/>
@@ -12134,14 +12157,8 @@
       <c r="L1024" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
+  <mergeCells count="24">
+    <mergeCell ref="D13:L20"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="A1:L2"/>
     <mergeCell ref="A4:C4"/>
@@ -12158,6 +12175,13 @@
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
tratando de alguns bug's da aplicação
</commit_message>
<xml_diff>
--- a/documentacao/dinheiroNoBolso.xlsx
+++ b/documentacao/dinheiroNoBolso.xlsx
@@ -125,19 +125,23 @@
     <t>DBRECEITADATARECEBIMENTO</t>
   </si>
   <si>
-    <r>
-      <t>DBDESPESATIPO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (Despesa Fixa = 0 e Variável = 1)</t>
-    </r>
+    <t>Script:                                                                                                                                                                                         CREATE TABLE `DBDESPESAS` (
+ `DBDESPESAID` INTEGER NOT NULL PRIMARY KEY AUTOINCREMENT,
+ `DBDESPESANOME` TEXT NOT NULL,
+ `DBDESPESATIPO` INTEGER NOT NULL,
+ `DBDESPESAVALOR` REAL NOT NULL,
+ `DBDESPESADATAVENC` TEXT NOT NULL,
+ `DBDESPESASTATUS` INTEGER NOT NULL
+);</t>
+  </si>
+  <si>
+    <t>Script:                                                                                                                                                                                         CREATE TABLE `DBRECEITAS` (
+ `DBRECEITAID` INTEGER NOT NULL PRIMARY KEY AUTOINCREMENT,
+ `DBRECEITANOME` TEXT NOT NULL,
+ `DBRECEITATIPO` INTEGER NOT NULL,
+ `DBRECEITAVALOR` REAL NOT NULL,
+ `DBRECEITADATARECEBIMENTO` TEXT NOT NULL
+);</t>
   </si>
   <si>
     <r>
@@ -151,18 +155,23 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(Despesa paga = 0 e à pagar = 1)</t>
+      <t>(Despesa paga = 1 e à pagar = 0)</t>
     </r>
   </si>
   <si>
-    <t>Script:                                                                                                                                                                                         CREATE TABLE `DBDESPESAS` (
- `DBDESPESAID` INTEGER NOT NULL PRIMARY KEY AUTOINCREMENT,
- `DBDESPESANOME` TEXT NOT NULL,
- `DBDESPESATIPO` INTEGER NOT NULL,
- `DBDESPESAVALOR` REAL NOT NULL,
- `DBDESPESADATAVENC` TEXT NOT NULL,
- `DBDESPESASTATUS` INTEGER NOT NULL
-);</t>
+    <r>
+      <t>DBDESPESATIPO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Despesa Fixa = 1) checkBox</t>
+    </r>
   </si>
   <si>
     <r>
@@ -176,17 +185,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(Receita Salário = 0 e Variável = 1)</t>
+      <t>(Receita Salário fixo = 1) checkBox</t>
     </r>
-  </si>
-  <si>
-    <t>Script:                                                                                                                                                                                         CREATE TABLE `DBRECEITAS` (
- `DBRECEITAID` INTEGER NOT NULL PRIMARY KEY AUTOINCREMENT,
- `DBRECEITANOME` TEXT NOT NULL,
- `DBRECEITATIPO` INTEGER NOT NULL,
- `DBRECEITAVALOR` REAL NOT NULL,
- `DBRECEITADATARECEBIMENTO` TEXT NOT NULL
-);</t>
   </si>
 </sst>
 </file>
@@ -275,11 +275,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -754,7 +754,7 @@
   <dimension ref="A1:L1024"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:C16"/>
+      <selection activeCell="B19" sqref="B19:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,8 +800,8 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
-      <c r="D3" s="12" t="s">
-        <v>38</v>
+      <c r="D3" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -813,11 +813,11 @@
       <c r="L3" s="9"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -887,7 +887,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="9"/>
@@ -941,7 +941,7 @@
         <v>29</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="9"/>
@@ -956,8 +956,8 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -974,8 +974,8 @@
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
-      <c r="D13" s="12" t="s">
-        <v>40</v>
+      <c r="D13" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
@@ -987,11 +987,11 @@
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -1061,7 +1061,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="9"/>
@@ -12174,14 +12174,14 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A14:C14"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementando a alteração da receita
</commit_message>
<xml_diff>
--- a/documentacao/dinheiroNoBolso.xlsx
+++ b/documentacao/dinheiroNoBolso.xlsx
@@ -270,13 +270,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -754,7 +754,7 @@
   <dimension ref="A1:L1024"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:C19"/>
+      <selection activeCell="B16" sqref="B16:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,52 +765,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -818,51 +818,51 @@
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -872,15 +872,15 @@
         <v>19</v>
       </c>
       <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -890,15 +890,15 @@
         <v>39</v>
       </c>
       <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -908,15 +908,15 @@
         <v>22</v>
       </c>
       <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -926,15 +926,15 @@
         <v>24</v>
       </c>
       <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -944,47 +944,47 @@
         <v>38</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
@@ -992,51 +992,51 @@
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -1046,15 +1046,15 @@
         <v>33</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -1064,51 +1064,51 @@
         <v>40</v>
       </c>
       <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D21" s="5"/>
@@ -1144,8 +1144,8 @@
       <c r="L23" s="5"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -1157,8 +1157,8 @@
       <c r="L24" s="5"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -1170,8 +1170,8 @@
       <c r="L25" s="5"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -12158,6 +12158,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
     <mergeCell ref="D13:L20"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="A1:L2"/>
@@ -12174,14 +12182,6 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A14:C14"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
adicionando funcionalidade as activity's finanças do mes, listar despesas vencidas e alterando plano de negócio da aplicação
</commit_message>
<xml_diff>
--- a/documentacao/dinheiroNoBolso.xlsx
+++ b/documentacao/dinheiroNoBolso.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>Projeto Dinheiro no Bolso (Aplicativo Android)</t>
   </si>
@@ -188,6 +188,9 @@
       <t>(Receita Salário fixo = 1) checkBox</t>
     </r>
   </si>
+  <si>
+    <t>Códigos Hexadecimais das cores ultilizadas no Aplicativo</t>
+  </si>
 </sst>
 </file>
 
@@ -270,13 +273,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -296,6 +299,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>185754</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>21981</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>85771</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="4567254"/>
+          <a:ext cx="4095750" cy="4853017"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -753,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1024"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:C16"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,52 +828,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="9" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -818,51 +881,51 @@
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -872,15 +935,15 @@
         <v>19</v>
       </c>
       <c r="C7" s="8"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -890,15 +953,15 @@
         <v>39</v>
       </c>
       <c r="C8" s="8"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -908,15 +971,15 @@
         <v>22</v>
       </c>
       <c r="C9" s="8"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -926,15 +989,15 @@
         <v>24</v>
       </c>
       <c r="C10" s="8"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -944,47 +1007,47 @@
         <v>38</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="9" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
@@ -992,33 +1055,33 @@
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -1028,15 +1091,15 @@
         <v>32</v>
       </c>
       <c r="C16" s="8"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -1046,15 +1109,15 @@
         <v>33</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -1064,15 +1127,15 @@
         <v>40</v>
       </c>
       <c r="C18" s="8"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
@@ -1082,15 +1145,15 @@
         <v>34</v>
       </c>
       <c r="C19" s="8"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
@@ -1100,17 +1163,22 @@
         <v>35</v>
       </c>
       <c r="C20" s="8"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -1122,6 +1190,9 @@
       <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -1133,6 +1204,9 @@
       <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -1144,8 +1218,9 @@
       <c r="L23" s="5"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -1157,8 +1232,8 @@
       <c r="L24" s="5"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -1170,8 +1245,8 @@
       <c r="L25" s="5"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -12158,14 +12233,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
     <mergeCell ref="D13:L20"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="A1:L2"/>
@@ -12182,8 +12249,17 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A14:C14"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="A21:C24"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>